<commit_message>
fixing beta_version.py / new code on ticket_management.py and main code for execute / v.11.9
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3401,6 +3401,100 @@
         </is>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>10:46:30</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>10:46:37</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>0:00:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>10:47:05</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Atasco tuerca</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>10:47:07</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new admin user / v.12
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3495,6 +3495,53 @@
         </is>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>10:51:43</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>10:52:50</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>0:01:07</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new button - refresh tickets / updating / v.12.7
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,7 +445,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -3541,6 +3540,307 @@
           <t>0:01:07</t>
         </is>
       </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>11:20:26</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>11:20:32</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>0:00:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>11:28:43</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>11:28:49</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>11:28:53</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>11:29:11</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Ascensor no sube</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>11:29:51</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>11:29:53</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>11:29:56</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>11:29:59</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>11:30:00</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update admin tickets / v.13
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -390,13 +390,25 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="9.5703125" customWidth="1" min="2" max="2"/>
+    <col width="27.7109375" customWidth="1" min="3" max="3"/>
+    <col width="31.85546875" customWidth="1" min="4" max="4"/>
+    <col width="30.85546875" customWidth="1" min="5" max="5"/>
+    <col width="21.42578125" customWidth="1" min="6" max="6"/>
+    <col width="35" customWidth="1" min="7" max="7"/>
+    <col width="26.28515625" customWidth="1" min="8" max="8"/>
+    <col width="27.85546875" customWidth="1" min="9" max="9"/>
+    <col width="27.5703125" customWidth="1" min="10" max="10"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -3839,8 +3851,317 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H77" t="inlineStr"/>
-      <c r="I77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>11:49:03</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>11:49:06</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>11:49:12</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>No atornilla tapa</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>11:51:03</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>11:52:16</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>0:01:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>12:07:13</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>12:07:15</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>12:08:05</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>12:08:08</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>12:16:49</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>12:16:52</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>12:18:27</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr"/>
+      <c r="I84" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixing beta_version.py  /  v.13
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4160,8 +4160,156 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H84" t="inlineStr"/>
-      <c r="I84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>13:43:58</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>13:44:52</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Tornillo atascado</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>13:58:53</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>14:24:33</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Ascensor no sube</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr"/>
+      <c r="I88" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixing advanced filter / fixing admin user / v.16
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -4308,8 +4309,1024 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H88" t="inlineStr"/>
-      <c r="I88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>09:25:35</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>09:25:42</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>0:00:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>09:25:44</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>No detecta presencia power CP</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>09:26:01</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>AOI (fallo etiqueta)</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>09:26:07</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>0:00:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>09:28:37</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>AOI no detecta pieza</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>09:28:48</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Ascensor no sube</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>09:28:57</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>0:00:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>09:28:59</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>09:29:04</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>0:00:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>09:29:32</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>09:29:37</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>0:00:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>09:36:37</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Core enganchado</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>09:37:53</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>09:39:42</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Top cover</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>09:42:43</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>09:43:11</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>09:49:24</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>No atornilla tapa</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>10:40:56</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>10:49:33</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foams</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>10:59:41</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>10:59:43</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>11:00:00</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Power CP</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>11:00:02</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>11:00:10</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foam derecho</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>11:00:12</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>11:00:14</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>11:00:43</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Tornillo atascado en tolva</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>11:00:45</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>11:02:27</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>11:02:28</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>11:06:41</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Cover atascado</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>11:06:48</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>0:00:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>11:09:15</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>11:09:17</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>11:10:39</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Fallo fijador tapa</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>11:10:40</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update ticket_management.py / v.16.5
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I112"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +457,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -5327,6 +5326,623 @@
           <t>0:00:01</t>
         </is>
       </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>11:13:02</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>11:13:05</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>11:17:09</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>11:21:58</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foams</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>11:22:01</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>No detecta presencia power CP</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>11:22:02</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>11:23:37</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>No atornilla tapa</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>11:23:43</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>11:25:58</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>No atornilla tapa</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>11:33:18</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>11:33:20</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>11:33:31</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>11:33:36</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>11:33:39</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>11:33:40</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>11:33:48</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>11:36:10</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Ascensor no sube</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>11:36:14</t>
+        </is>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>11:36:16</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>AOI no detecta pieza</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>11:36:18</t>
+        </is>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>11:36:20</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Fallo fijador tapa</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr"/>
+      <c r="I127" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
correcting issues / v.17
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:I131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -5941,8 +5942,184 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H127" t="inlineStr"/>
-      <c r="I127" t="inlineStr"/>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>11:42:31</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>11:42:35</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Ascensor no sube</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>11:42:37</t>
+        </is>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>11:43:12</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>AOI (malla)</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>11:43:14</t>
+        </is>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>11:43:16</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foams</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>11:43:18</t>
+        </is>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
error fixed / buttons running perfectly / v.17
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I131"/>
+  <dimension ref="A1:I135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6121,6 +6121,194 @@
         </is>
       </c>
     </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>11:50:30</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>11:50:32</t>
+        </is>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>11:50:35</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>11:50:42</t>
+        </is>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>0:00:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>11:50:39</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>11:50:40</t>
+        </is>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>11:51:29</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>11:51:31</t>
+        </is>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update admin_dialog.py / v.20
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:I136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6309,6 +6309,53 @@
         </is>
       </c>
     </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>11:53:25</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Secuencia atornillador</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>11:53:26</t>
+        </is>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
admin_dialog.py FIXED / v.21
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I136"/>
+  <dimension ref="A1:I139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6356,6 +6356,147 @@
         </is>
       </c>
     </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>12:03:58</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>12:06:11</t>
+        </is>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>0:02:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>12:09:37</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Etiquetadora2</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>12:09:39</t>
+        </is>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>12:10:19</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>12:10:20</t>
+        </is>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
loading json for tickets update from admin user modifications / v.21
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I139"/>
+  <dimension ref="A1:I142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6497,6 +6497,147 @@
         </is>
       </c>
     </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>12:17:26</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Etiquetadora2</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>12:17:28</t>
+        </is>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>12:22:15</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Etiquetadora2</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>12:22:17</t>
+        </is>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>12:23:29</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>12:23:31</t>
+        </is>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update admin_dialog.py / tickets modified are totally implemented in the other users / v.21
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I142"/>
+  <dimension ref="A1:I144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6638,6 +6638,100 @@
         </is>
       </c>
     </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>12:35:19</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>12:35:21</t>
+        </is>
+      </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>12:36:05</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Etiquetadora21212</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>12:36:06</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update admin_dialog.py and ticket_management.py / new excel window interface  /  admin permissions fixed / table update / v.25
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I144"/>
+  <dimension ref="A1:I146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6732,6 +6732,100 @@
         </is>
       </c>
     </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>12:50:41</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>12:50:44</t>
+        </is>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>12:58:21</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Etiquetadora21212</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>12:58:26</t>
+        </is>
+      </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>0:00:05</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new excel_window.py / updating ticket_manegement.py / v.25
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I146"/>
+  <dimension ref="A1:I151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6826,6 +6826,241 @@
         </is>
       </c>
     </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>09:24:06</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>09:24:08</t>
+        </is>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>09:24:18</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>09:24:19</t>
+        </is>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>09:26:52</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>09:26:53</t>
+        </is>
+      </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>09:37:40</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>09:37:46</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>0:00:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>09:37:44</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>09:37:48</t>
+        </is>
+      </c>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
excel view new interface / better update / v.25.5
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I151"/>
+  <dimension ref="A1:I154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +457,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -7060,6 +7059,129 @@
           <t>0:00:04</t>
         </is>
       </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>09:51:09</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>09:51:13</t>
+        </is>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>09:58:36</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Fallo fijador tapa</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>10:04:21</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien ferrita</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr"/>
+      <c r="I154" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new file / incidence_chart.py / new graph and fixing ticket_management.py / v.25.8
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I154"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -7180,8 +7181,194 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H154" t="inlineStr"/>
-      <c r="I154" t="inlineStr"/>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>10:31:45</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>NOK Soldadura metal</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>10:31:48</t>
+        </is>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>10:38:28</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>Colisión placas</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>10:38:30</t>
+        </is>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>10:38:44</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>Fallo dispensación glue</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>10:38:47</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>10:38:49</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>Error en sensor de salida</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>10:39:53</t>
+        </is>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>0:01:04</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixing graph and excel_window / incidence_chart / v.26
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I158"/>
+  <dimension ref="A1:I159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +457,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -7369,6 +7368,45 @@
           <t>0:01:04</t>
         </is>
       </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>11:12:43</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>NOK Soldadura metal</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr"/>
+      <c r="I159" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
error fixed / updating principal graph / v.27
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I159"/>
+  <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -7405,8 +7406,241 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H159" t="inlineStr"/>
-      <c r="I159" t="inlineStr"/>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>11:22:43</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>11:22:51</t>
+        </is>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>0:00:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>11:22:53</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>No atornilla tapa</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>11:22:56</t>
+        </is>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>11:23:21</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>11:23:35</t>
+        </is>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>0:00:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>11:25:01</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Fallo en elevador_3</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>11:25:03</t>
+        </is>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>11:25:42</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Fallo en elevador_3</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>11:25:43</t>
+        </is>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating graph / v.27.8
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I164"/>
+  <dimension ref="A1:I168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7642,6 +7642,194 @@
         </is>
       </c>
     </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>11:27:04</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foams</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>11:27:47</t>
+        </is>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>0:00:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>11:32:21</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>AOI (fallo etiqueta)</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>11:32:27</t>
+        </is>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>0:00:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>11:32:25</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foam derecho</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>11:32:29</t>
+        </is>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>11:35:54</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>AOI (fallo etiqueta)</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>11:35:59</t>
+        </is>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>0:00:05</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
graph updated / v.30
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I168"/>
+  <dimension ref="A1:I181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7830,6 +7830,617 @@
         </is>
       </c>
     </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>11:48:35</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Top Cover</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>11:48:43</t>
+        </is>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>0:00:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>11:48:47</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>11:48:48</t>
+        </is>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>11:51:01</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>Marco atascado en parte inferior</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>11:51:05</t>
+        </is>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>11:51:07</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>No detecta marcas Power</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>11:51:10</t>
+        </is>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>11:53:26</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>11:53:33</t>
+        </is>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>0:00:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>11:53:35</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>11:53:39</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>11:54:07</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>11:54:12</t>
+        </is>
+      </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>0:00:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>11:54:10</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foam derecho</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>11:54:14</t>
+        </is>
+      </c>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>11:54:51</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foams</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>11:54:53</t>
+        </is>
+      </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>11:54:56</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>11:55:00</t>
+        </is>
+      </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>11:55:35</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>11:55:37</t>
+        </is>
+      </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>11:56:09</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foam derecho</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>11:56:10</t>
+        </is>
+      </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>11:56:15</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>AOI (malla)</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>11:56:16</t>
+        </is>
+      </c>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more ideas / text.txt
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I181"/>
+  <dimension ref="A1:I186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8441,6 +8441,231 @@
         </is>
       </c>
     </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>12:02:22</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>Fallo en elevador_2</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>12:02:23</t>
+        </is>
+      </c>
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>12:07:33</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>12:07:40</t>
+        </is>
+      </c>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>0:00:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>12:07:37</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>12:07:41</t>
+        </is>
+      </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>12:07:59</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>12:08:28</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H186" t="inlineStr">
+        <is>
+          <t>12:08:31</t>
+        </is>
+      </c>
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixing and implementing new ideas / v.30.2
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I186"/>
+  <dimension ref="A1:I189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8666,6 +8666,147 @@
         </is>
       </c>
     </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>12:13:36</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>Etiquetadora_2</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>12:13:38</t>
+        </is>
+      </c>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>12:18:13</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>12:18:30</t>
+        </is>
+      </c>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>0:00:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>12:43:29</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Ascensor no sube</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>12:43:32</t>
+        </is>
+      </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
waiting for fix ticket_management / v.35
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I189"/>
+  <dimension ref="A1:I191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8807,6 +8807,90 @@
         </is>
       </c>
     </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>14:51:00</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foams</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>2024-05-22</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>15:35:13</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>15:35:15</t>
+        </is>
+      </c>
+      <c r="I191" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixing turn chart / principal graph / v.38
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I191"/>
+  <dimension ref="A1:I196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +457,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -8890,6 +8889,233 @@
           <t>0:00:02</t>
         </is>
       </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>09:26:36</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H192" t="inlineStr">
+        <is>
+          <t>09:26:40</t>
+        </is>
+      </c>
+      <c r="I192" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>09:34:23</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>No coloca bien el sealling</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>09:34:25</t>
+        </is>
+      </c>
+      <c r="I193" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>09:42:46</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien filter en palet</t>
+        </is>
+      </c>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H194" t="inlineStr">
+        <is>
+          <t>09:42:48</t>
+        </is>
+      </c>
+      <c r="I194" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>09:42:50</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>NOK Soldadura Plástico</t>
+        </is>
+      </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>09:42:52</t>
+        </is>
+      </c>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>09:42:53</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>Pieza enganchada en HV Test</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H196" t="inlineStr"/>
+      <c r="I196" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
graph update / new buttons for two graphs / fixing / v.40
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I196"/>
+  <dimension ref="A1:I209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -9114,8 +9115,597 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H196" t="inlineStr"/>
-      <c r="I196" t="inlineStr"/>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>09:49:58</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foam derecho</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>09:50:12</t>
+        </is>
+      </c>
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>0:00:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>09:50:39</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>AOI (malla)</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>09:50:42</t>
+        </is>
+      </c>
+      <c r="I198" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>10:39:08</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>10:41:53</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>10:41:59</t>
+        </is>
+      </c>
+      <c r="I200" t="inlineStr">
+        <is>
+          <t>0:00:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>10:42:21</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>10:42:30</t>
+        </is>
+      </c>
+      <c r="I201" t="inlineStr">
+        <is>
+          <t>0:00:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>10:42:33</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>No detecta presencia power CP</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H202" t="inlineStr">
+        <is>
+          <t>10:42:36</t>
+        </is>
+      </c>
+      <c r="I202" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>10:46:15</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foam derecho</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>10:46:17</t>
+        </is>
+      </c>
+      <c r="I203" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>10:48:22</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>Colisión placas</t>
+        </is>
+      </c>
+      <c r="H204" t="inlineStr">
+        <is>
+          <t>10:48:25</t>
+        </is>
+      </c>
+      <c r="I204" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>10:48:26</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>Soldadura defectuosa</t>
+        </is>
+      </c>
+      <c r="H205" t="inlineStr">
+        <is>
+          <t>10:48:28</t>
+        </is>
+      </c>
+      <c r="I205" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>11:36:30</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>11:39:40</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H207" t="inlineStr">
+        <is>
+          <t>11:40:25</t>
+        </is>
+      </c>
+      <c r="I207" t="inlineStr">
+        <is>
+          <t>0:00:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>11:57:13</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>11:57:24</t>
+        </is>
+      </c>
+      <c r="I208" t="inlineStr">
+        <is>
+          <t>0:00:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>11:57:20</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H209" t="inlineStr">
+        <is>
+          <t>11:57:24</t>
+        </is>
+      </c>
+      <c r="I209" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
graphs updated / fix / v.40
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I209"/>
+  <dimension ref="A1:I211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9707,6 +9707,100 @@
         </is>
       </c>
     </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>12:11:48</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H210" t="inlineStr">
+        <is>
+          <t>12:11:49</t>
+        </is>
+      </c>
+      <c r="I210" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>12:14:05</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H211" t="inlineStr">
+        <is>
+          <t>12:14:07</t>
+        </is>
+      </c>
+      <c r="I211" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
implementing MTBF / v.40.5
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I211"/>
+  <dimension ref="A1:I222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9801,6 +9801,473 @@
         </is>
       </c>
     </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>12:23:32</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>12:23:35</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Top Cover</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>12:23:37</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>12:23:41</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>12:23:43</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G216" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>12:29:02</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien filter en palet</t>
+        </is>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>12:29:06</t>
+        </is>
+      </c>
+      <c r="I217" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>12:29:07</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien filter en palet</t>
+        </is>
+      </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H218" t="inlineStr">
+        <is>
+          <t>12:29:10</t>
+        </is>
+      </c>
+      <c r="I218" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>12:29:11</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="G219" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H219" t="inlineStr">
+        <is>
+          <t>12:29:13</t>
+        </is>
+      </c>
+      <c r="I219" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>12:29:16</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>Fallo cámara ferrite</t>
+        </is>
+      </c>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H220" t="inlineStr">
+        <is>
+          <t>12:33:55</t>
+        </is>
+      </c>
+      <c r="I220" t="inlineStr">
+        <is>
+          <t>0:04:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>12:30:05</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>Pieza enganchada en HV Test</t>
+        </is>
+      </c>
+      <c r="G221" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H221" t="inlineStr">
+        <is>
+          <t>12:33:54</t>
+        </is>
+      </c>
+      <c r="I221" t="inlineStr">
+        <is>
+          <t>0:03:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>12:32:36</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>Fallo Funcional</t>
+        </is>
+      </c>
+      <c r="G222" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H222" t="inlineStr">
+        <is>
+          <t>12:33:53</t>
+        </is>
+      </c>
+      <c r="I222" t="inlineStr">
+        <is>
+          <t>0:01:17</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixing MTBF / not working / v.50
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I222"/>
+  <dimension ref="A1:I237"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +457,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -10267,6 +10266,703 @@
           <t>0:01:17</t>
         </is>
       </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>12:44:53</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H223" t="inlineStr">
+        <is>
+          <t>12:47:11</t>
+        </is>
+      </c>
+      <c r="I223" t="inlineStr">
+        <is>
+          <t>0:02:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>12:44:57</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Top cover</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G224" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H224" t="inlineStr">
+        <is>
+          <t>12:47:12</t>
+        </is>
+      </c>
+      <c r="I224" t="inlineStr">
+        <is>
+          <t>0:02:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>12:45:02</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G225" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H225" t="inlineStr">
+        <is>
+          <t>12:47:10</t>
+        </is>
+      </c>
+      <c r="I225" t="inlineStr">
+        <is>
+          <t>0:02:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>12:45:05</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>No detecta presencia power CP</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G226" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H226" t="inlineStr">
+        <is>
+          <t>12:47:10</t>
+        </is>
+      </c>
+      <c r="I226" t="inlineStr">
+        <is>
+          <t>0:02:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>12:45:15</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G227" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H227" t="inlineStr">
+        <is>
+          <t>12:47:09</t>
+        </is>
+      </c>
+      <c r="I227" t="inlineStr">
+        <is>
+          <t>0:01:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>12:45:59</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G228" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H228" t="inlineStr">
+        <is>
+          <t>12:47:08</t>
+        </is>
+      </c>
+      <c r="I228" t="inlineStr">
+        <is>
+          <t>0:01:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>12:46:01</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G229" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H229" t="inlineStr">
+        <is>
+          <t>12:47:07</t>
+        </is>
+      </c>
+      <c r="I229" t="inlineStr">
+        <is>
+          <t>0:01:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>12:47:04</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G230" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H230" t="inlineStr">
+        <is>
+          <t>12:47:05</t>
+        </is>
+      </c>
+      <c r="I230" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>12:50:44</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foam derecho</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G231" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H231" t="inlineStr">
+        <is>
+          <t>12:51:15</t>
+        </is>
+      </c>
+      <c r="I231" t="inlineStr">
+        <is>
+          <t>0:00:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>12:54:54</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G232" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H232" t="inlineStr">
+        <is>
+          <t>12:58:51</t>
+        </is>
+      </c>
+      <c r="I232" t="inlineStr">
+        <is>
+          <t>0:03:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>12:55:18</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>AOI (fallo etiqueta)</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G233" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H233" t="inlineStr">
+        <is>
+          <t>12:58:53</t>
+        </is>
+      </c>
+      <c r="I233" t="inlineStr">
+        <is>
+          <t>0:03:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>12:55:21</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G234" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H234" t="inlineStr">
+        <is>
+          <t>12:58:54</t>
+        </is>
+      </c>
+      <c r="I234" t="inlineStr">
+        <is>
+          <t>0:03:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>13:00:11</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>Robot no coge busbar</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G235" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H235" t="inlineStr">
+        <is>
+          <t>13:00:15</t>
+        </is>
+      </c>
+      <c r="I235" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>13:00:22</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>Robot no coge busbar</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G236" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H236" t="inlineStr">
+        <is>
+          <t>13:00:23</t>
+        </is>
+      </c>
+      <c r="I236" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>13:01:41</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G237" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H237" t="inlineStr"/>
+      <c r="I237" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
app working succesuflly / v.45
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I237"/>
+  <dimension ref="A1:I241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -10961,8 +10962,174 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H237" t="inlineStr"/>
-      <c r="I237" t="inlineStr"/>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>15:21:03</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G238" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>15:33:56</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G239" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H239" t="inlineStr">
+        <is>
+          <t>15:33:59</t>
+        </is>
+      </c>
+      <c r="I239" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>15:34:01</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G240" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>15:36:48</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="G241" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H241" t="inlineStr">
+        <is>
+          <t>15:36:49</t>
+        </is>
+      </c>
+      <c r="I241" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
info add on button / v.50
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I241"/>
+  <dimension ref="A1:I243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11131,6 +11131,100 @@
         </is>
       </c>
     </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>15:53:35</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foam derecho</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G242" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H242" t="inlineStr">
+        <is>
+          <t>15:53:40</t>
+        </is>
+      </c>
+      <c r="I242" t="inlineStr">
+        <is>
+          <t>0:00:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>15:53:37</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>AOI (malla)</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G243" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H243" t="inlineStr">
+        <is>
+          <t>15:53:41</t>
+        </is>
+      </c>
+      <c r="I243" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new interface /& v.50.5
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I243"/>
+  <dimension ref="A1:I247"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11225,6 +11225,194 @@
         </is>
       </c>
     </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>16:04:35</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G244" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H244" t="inlineStr">
+        <is>
+          <t>16:04:37</t>
+        </is>
+      </c>
+      <c r="I244" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>16:04:39</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>Fallo tolva</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F245" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G245" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H245" t="inlineStr">
+        <is>
+          <t>16:05:06</t>
+        </is>
+      </c>
+      <c r="I245" t="inlineStr">
+        <is>
+          <t>0:00:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>16:24:50</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G246" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H246" t="inlineStr">
+        <is>
+          <t>16:24:51</t>
+        </is>
+      </c>
+      <c r="I246" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>2024-05-23</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>16:24:53</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G247" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H247" t="inlineStr">
+        <is>
+          <t>16:24:54</t>
+        </is>
+      </c>
+      <c r="I247" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new modalities and interface update for all / new icon / adv filter fixed and details / v.60
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I247"/>
+  <dimension ref="A1:I270"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11413,6 +11413,1087 @@
         </is>
       </c>
     </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>09:27:03</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>Atasco tuerca</t>
+        </is>
+      </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G248" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H248" t="inlineStr">
+        <is>
+          <t>09:27:05</t>
+        </is>
+      </c>
+      <c r="I248" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>09:32:36</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>No coloca bien el sealling</t>
+        </is>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G249" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H249" t="inlineStr">
+        <is>
+          <t>09:33:41</t>
+        </is>
+      </c>
+      <c r="I249" t="inlineStr">
+        <is>
+          <t>0:01:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>09:34:21</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G250" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H250" t="inlineStr">
+        <is>
+          <t>09:34:33</t>
+        </is>
+      </c>
+      <c r="I250" t="inlineStr">
+        <is>
+          <t>0:00:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>09:35:20</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>No coloca bien el sealling</t>
+        </is>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G251" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H251" t="inlineStr">
+        <is>
+          <t>09:35:21</t>
+        </is>
+      </c>
+      <c r="I251" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>09:40:07</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G252" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H252" t="inlineStr">
+        <is>
+          <t>09:40:09</t>
+        </is>
+      </c>
+      <c r="I252" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>09:40:10</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>No lee QR</t>
+        </is>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G253" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H253" t="inlineStr">
+        <is>
+          <t>09:40:11</t>
+        </is>
+      </c>
+      <c r="I253" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>09:40:50</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F254" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G254" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H254" t="inlineStr">
+        <is>
+          <t>09:40:52</t>
+        </is>
+      </c>
+      <c r="I254" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>09:41:05</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G255" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H255" t="inlineStr">
+        <is>
+          <t>09:41:07</t>
+        </is>
+      </c>
+      <c r="I255" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>09:42:11</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>Robot no coge busbar</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G256" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H256" t="inlineStr">
+        <is>
+          <t>09:42:13</t>
+        </is>
+      </c>
+      <c r="I256" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>09:45:30</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="G257" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H257" t="inlineStr">
+        <is>
+          <t>09:45:32</t>
+        </is>
+      </c>
+      <c r="I257" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>09:45:34</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>No coloca bien la pcb</t>
+        </is>
+      </c>
+      <c r="G258" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H258" t="inlineStr">
+        <is>
+          <t>09:45:35</t>
+        </is>
+      </c>
+      <c r="I258" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>09:45:39</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="G259" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H259" t="inlineStr">
+        <is>
+          <t>09:45:41</t>
+        </is>
+      </c>
+      <c r="I259" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>09:46:53</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>NOK Soldad. Plástico+Metal</t>
+        </is>
+      </c>
+      <c r="G260" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H260" t="inlineStr">
+        <is>
+          <t>09:46:56</t>
+        </is>
+      </c>
+      <c r="I260" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>09:47:37</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>Fallo cámara ferrite</t>
+        </is>
+      </c>
+      <c r="G261" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H261" t="inlineStr">
+        <is>
+          <t>09:47:39</t>
+        </is>
+      </c>
+      <c r="I261" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>09:49:35</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>Robot no coge PCB</t>
+        </is>
+      </c>
+      <c r="G262" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H262" t="inlineStr">
+        <is>
+          <t>09:49:37</t>
+        </is>
+      </c>
+      <c r="I262" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>09:50:22</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>NOK Soldad. Plástico+Metal</t>
+        </is>
+      </c>
+      <c r="G263" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H263" t="inlineStr">
+        <is>
+          <t>09:50:25</t>
+        </is>
+      </c>
+      <c r="I263" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>09:53:36</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>Tornillo atascado en tolva</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G264" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H264" t="inlineStr">
+        <is>
+          <t>09:53:43</t>
+        </is>
+      </c>
+      <c r="I264" t="inlineStr">
+        <is>
+          <t>0:00:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>09:53:44</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G265" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H265" t="inlineStr">
+        <is>
+          <t>09:53:46</t>
+        </is>
+      </c>
+      <c r="I265" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>09:54:11</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G266" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H266" t="inlineStr">
+        <is>
+          <t>09:54:12</t>
+        </is>
+      </c>
+      <c r="I266" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>09:54:40</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G267" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H267" t="inlineStr">
+        <is>
+          <t>09:54:41</t>
+        </is>
+      </c>
+      <c r="I267" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>10:40:39</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F268" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G268" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H268" t="inlineStr">
+        <is>
+          <t>10:40:40</t>
+        </is>
+      </c>
+      <c r="I268" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>11:02:33</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G269" t="inlineStr">
+        <is>
+          <t>Fallo dispensación glue</t>
+        </is>
+      </c>
+      <c r="H269" t="inlineStr">
+        <is>
+          <t>11:02:36</t>
+        </is>
+      </c>
+      <c r="I269" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>11:02:35</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F270" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G270" t="inlineStr">
+        <is>
+          <t>Error en sensor de salida</t>
+        </is>
+      </c>
+      <c r="H270" t="inlineStr">
+        <is>
+          <t>11:02:36</t>
+        </is>
+      </c>
+      <c r="I270" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new graph update and fixing some issues / better funcionality /v.60.7
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I270"/>
+  <dimension ref="A1:I275"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12494,6 +12494,241 @@
         </is>
       </c>
     </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>11:58:29</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G271" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H271" t="inlineStr">
+        <is>
+          <t>11:58:31</t>
+        </is>
+      </c>
+      <c r="I271" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>11:59:54</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>Atasco tuerca</t>
+        </is>
+      </c>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G272" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H272" t="inlineStr">
+        <is>
+          <t>11:59:57</t>
+        </is>
+      </c>
+      <c r="I272" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>12:32:55</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G273" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H273" t="inlineStr">
+        <is>
+          <t>12:33:26</t>
+        </is>
+      </c>
+      <c r="I273" t="inlineStr">
+        <is>
+          <t>0:00:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>12:46:31</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G274" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H274" t="inlineStr">
+        <is>
+          <t>12:46:35</t>
+        </is>
+      </c>
+      <c r="I274" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>12:46:36</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>No atornilla tapa</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G275" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H275" t="inlineStr">
+        <is>
+          <t>12:46:38</t>
+        </is>
+      </c>
+      <c r="I275" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
graphs updated / json file charging complete / v.7.0
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I275"/>
+  <dimension ref="A1:I286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12729,6 +12729,523 @@
         </is>
       </c>
     </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>10:51:31</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>Cámara no detecta busbar</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F276" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G276" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H276" t="inlineStr">
+        <is>
+          <t>10:51:33</t>
+        </is>
+      </c>
+      <c r="I276" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>10:51:51</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>No detecta presencia power CP</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G277" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H277" t="inlineStr">
+        <is>
+          <t>10:51:53</t>
+        </is>
+      </c>
+      <c r="I277" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>10:52:01</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G278" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H278" t="inlineStr">
+        <is>
+          <t>10:52:03</t>
+        </is>
+      </c>
+      <c r="I278" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>10:52:06</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G279" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H279" t="inlineStr">
+        <is>
+          <t>10:52:08</t>
+        </is>
+      </c>
+      <c r="I279" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>10:54:19</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foams</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G280" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H280" t="inlineStr">
+        <is>
+          <t>10:54:21</t>
+        </is>
+      </c>
+      <c r="I280" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>10:54:24</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foams</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G281" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H281" t="inlineStr">
+        <is>
+          <t>10:54:26</t>
+        </is>
+      </c>
+      <c r="I281" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>10:56:29</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>No coloca bien el sealling</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G282" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H282" t="inlineStr">
+        <is>
+          <t>10:56:32</t>
+        </is>
+      </c>
+      <c r="I282" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>11:12:33</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>No coloca bien el sealling</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G283" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H283" t="inlineStr">
+        <is>
+          <t>11:12:36</t>
+        </is>
+      </c>
+      <c r="I283" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>11:12:38</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Cámara no detecta busbar</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G284" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H284" t="inlineStr">
+        <is>
+          <t>11:12:40</t>
+        </is>
+      </c>
+      <c r="I284" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>11:24:06</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G285" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H285" t="inlineStr">
+        <is>
+          <t>11:24:09</t>
+        </is>
+      </c>
+      <c r="I285" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>11:24:12</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Power CP</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G286" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H286" t="inlineStr">
+        <is>
+          <t>11:24:14</t>
+        </is>
+      </c>
+      <c r="I286" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
mtbf method updated and fixed / v.8
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I286"/>
+  <dimension ref="A1:I299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13246,6 +13246,617 @@
         </is>
       </c>
     </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>11:28:58</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>Screw K30 no lo detecta puesto</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G287" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H287" t="inlineStr">
+        <is>
+          <t>11:29:04</t>
+        </is>
+      </c>
+      <c r="I287" t="inlineStr">
+        <is>
+          <t>0:00:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>11:29:03</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>No lee QR</t>
+        </is>
+      </c>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G288" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H288" t="inlineStr">
+        <is>
+          <t>11:29:04</t>
+        </is>
+      </c>
+      <c r="I288" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>11:29:06</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G289" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H289" t="inlineStr">
+        <is>
+          <t>11:29:08</t>
+        </is>
+      </c>
+      <c r="I289" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>11:29:24</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Top Cover</t>
+        </is>
+      </c>
+      <c r="F290" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G290" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H290" t="inlineStr">
+        <is>
+          <t>11:29:26</t>
+        </is>
+      </c>
+      <c r="I290" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>11:29:27</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>No lee QR</t>
+        </is>
+      </c>
+      <c r="F291" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G291" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H291" t="inlineStr">
+        <is>
+          <t>11:29:28</t>
+        </is>
+      </c>
+      <c r="I291" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>11:29:29</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="F292" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G292" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H292" t="inlineStr">
+        <is>
+          <t>11:29:31</t>
+        </is>
+      </c>
+      <c r="I292" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>11:29:37</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G293" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H293" t="inlineStr">
+        <is>
+          <t>11:29:41</t>
+        </is>
+      </c>
+      <c r="I293" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>11:29:40</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Top Cover</t>
+        </is>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G294" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H294" t="inlineStr">
+        <is>
+          <t>11:29:41</t>
+        </is>
+      </c>
+      <c r="I294" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>11:40:49</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foams</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F295" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G295" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H295" t="inlineStr">
+        <is>
+          <t>11:40:52</t>
+        </is>
+      </c>
+      <c r="I295" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>11:40:53</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Power CP</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G296" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H296" t="inlineStr">
+        <is>
+          <t>11:40:55</t>
+        </is>
+      </c>
+      <c r="I296" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>11:41:47</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>Atasco tuerca</t>
+        </is>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G297" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H297" t="inlineStr">
+        <is>
+          <t>11:41:52</t>
+        </is>
+      </c>
+      <c r="I297" t="inlineStr">
+        <is>
+          <t>0:00:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>11:41:50</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>No lee QR</t>
+        </is>
+      </c>
+      <c r="F298" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G298" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H298" t="inlineStr">
+        <is>
+          <t>11:41:51</t>
+        </is>
+      </c>
+      <c r="I298" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>11:41:53</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G299" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H299" t="inlineStr">
+        <is>
+          <t>11:41:55</t>
+        </is>
+      </c>
+      <c r="I299" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
UI updating / new code structure / new files / v.9
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/tickets_pideu.xlsx
+++ b/beta_version/excel_files/tickets_pideu.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I299"/>
+  <dimension ref="A1:I308"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13857,6 +13857,429 @@
         </is>
       </c>
     </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>11:48:23</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G300" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H300" t="inlineStr">
+        <is>
+          <t>11:48:26</t>
+        </is>
+      </c>
+      <c r="I300" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>11:48:27</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>No coloca bien el sealling</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G301" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H301" t="inlineStr">
+        <is>
+          <t>11:48:29</t>
+        </is>
+      </c>
+      <c r="I301" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>12:13:45</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien filter en palet</t>
+        </is>
+      </c>
+      <c r="G302" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H302" t="inlineStr">
+        <is>
+          <t>12:13:47</t>
+        </is>
+      </c>
+      <c r="I302" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>12:14:07</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>NOK Soldadura metal</t>
+        </is>
+      </c>
+      <c r="G303" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H303" t="inlineStr">
+        <is>
+          <t>12:14:08</t>
+        </is>
+      </c>
+      <c r="I303" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>12:14:24</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien filter en palet</t>
+        </is>
+      </c>
+      <c r="G304" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H304" t="inlineStr">
+        <is>
+          <t>12:14:28</t>
+        </is>
+      </c>
+      <c r="I304" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>12:14:26</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien filter en palet</t>
+        </is>
+      </c>
+      <c r="G305" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H305" t="inlineStr">
+        <is>
+          <t>12:14:28</t>
+        </is>
+      </c>
+      <c r="I305" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>12:14:33</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien filter en palet</t>
+        </is>
+      </c>
+      <c r="G306" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H306" t="inlineStr">
+        <is>
+          <t>12:14:35</t>
+        </is>
+      </c>
+      <c r="I306" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>12:46:23</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G307" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H307" t="inlineStr">
+        <is>
+          <t>12:46:25</t>
+        </is>
+      </c>
+      <c r="I307" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>2024-05-27</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>12:46:28</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>Cámara no detecta busbar</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G308" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H308" t="inlineStr">
+        <is>
+          <t>12:46:30</t>
+        </is>
+      </c>
+      <c r="I308" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>